<commit_message>
Unit tests and fmt
</commit_message>
<xml_diff>
--- a/mock/migration/data.xlsx
+++ b/mock/migration/data.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Go XLSX"/>
-  <workbookPr showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Documents\_Workspace\go\src\github.com\andreluzz\cas-xog\mock\migration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="204"/>
   </bookViews>
   <sheets>
-    <sheet name="Instances" sheetId="1" r:id="rId1" state="visible"/>
+    <sheet name="Instances" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr iterateCount="100" refMode="A1" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>S0000001</t>
   </si>
@@ -31,47 +34,67 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>S0000002</t>
+  </si>
+  <si>
+    <t>S0000003</t>
+  </si>
+  <si>
+    <t>CAL_IN_PROGRESS</t>
+  </si>
+  <si>
+    <t>CAL_CLOSED;CAL_DONE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
-      <family val="0"/>
-      <charset val="0"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="00000000"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,26 +419,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.5"/>
+    <col min="1" max="1" width="9.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,11 +452,42 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>